<commit_message>
dev: colocado dados e feito grafico exemplo
</commit_message>
<xml_diff>
--- a/controle_estoque/controle_estoque.xlsx
+++ b/controle_estoque/controle_estoque.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clodo\OneDrive\Documentos\projetos_excel\controle_estoque\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D9141D-4C78-45B0-8ABB-CF98548D5346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B34CA5-2777-4A35-8446-50F05458368C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
     <sheet name="cadastro" sheetId="3" r:id="rId2"/>
     <sheet name="lancamento" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="cluna_produtos">tb_cadastro[Produto]</definedName>
+    <definedName name="coluna_produtos">tb_cadastro[Produto]</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Produto</t>
   </si>
@@ -78,12 +82,18 @@
   <si>
     <t>entrada</t>
   </si>
+  <si>
+    <t>Corretivo</t>
+  </si>
+  <si>
+    <t>Por que essas formulas todas? Porcausa que estamos calculando o saldo a cada lançamento</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +116,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +162,39 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -141,11 +205,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -162,11 +229,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -178,13 +241,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
+    <cellStyle name="Ênfase1" xfId="4" builtinId="29"/>
+    <cellStyle name="Neutro" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ruim" xfId="2" builtinId="27"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
+  <dxfs count="40">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -194,6 +296,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -204,6 +316,98 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
@@ -221,6 +425,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -250,7 +455,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -260,7 +464,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -300,7 +503,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -310,7 +512,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -320,7 +521,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -330,6 +538,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -339,6 +548,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -348,9 +558,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -378,31 +585,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -427,6 +610,1077 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Composição</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Atual do Estoque</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cadastro!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Saldo </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-9D6A-42B3-A76E-AC4466410150}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-9D6A-42B3-A76E-AC4466410150}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-9D6A-42B3-A76E-AC4466410150}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9D6A-42B3-A76E-AC4466410150}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-9D6A-42B3-A76E-AC4466410150}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.6939494688137957E-2"/>
+                  <c:y val="5.3215065217553134E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-9D6A-42B3-A76E-AC4466410150}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5306442083616869E-2"/>
+                  <c:y val="0.11234291545927907"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-9D6A-42B3-A76E-AC4466410150}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.6888094713842937E-2"/>
+                  <c:y val="-4.1389495169208187E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-9D6A-42B3-A76E-AC4466410150}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.321470523474717E-2"/>
+                  <c:y val="-0.11529930797136535"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-9D6A-42B3-A76E-AC4466410150}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4286273646329519E-2"/>
+                  <c:y val="-7.9822597826329875E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-9D6A-42B3-A76E-AC4466410150}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>cadastro!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Caneta esferográfica azul</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Caneta esferográfica preta</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Caneta esferográfica vermelha</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apontador</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Corretivo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cadastro!$E$4:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9D6A-42B3-A76E-AC4466410150}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1072,6 +2326,42 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>8286751</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2163E0F-4D47-4E60-8C69-7CB1A97A6ABE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1325,29 +2615,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8E0D29C-C5C8-419E-8C6A-D7DC69C44BB1}" name="tb_cadastro" displayName="tb_cadastro" ref="A3:F8" totalsRowCount="1" headerRowDxfId="25" dataDxfId="21" headerRowCellStyle="Bom">
-  <autoFilter ref="A3:F7" xr:uid="{C8E0D29C-C5C8-419E-8C6A-D7DC69C44BB1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8E0D29C-C5C8-419E-8C6A-D7DC69C44BB1}" name="tb_cadastro" displayName="tb_cadastro" ref="A3:F9" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38" headerRowCellStyle="Bom">
+  <autoFilter ref="A3:F8" xr:uid="{C8E0D29C-C5C8-419E-8C6A-D7DC69C44BB1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{06F20511-43B0-4213-B039-8F04FE3FD409}" name="Produto" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{833D9E07-786D-4F11-ADBE-EB9FE9DA20F3}" name="Medida" dataDxfId="23" totalsRowDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{2E7F5760-F579-440C-BB90-F0ABAA3977A1}" name="Estoque _x000a_Minimo" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{3544D7B8-7225-4D56-B67E-FCBE646D64FA}" name="Estoque _x000a_maximo" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{941540F3-D296-4F60-96B3-0CA20F164402}" name="Saldo " totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{28ED0648-8C45-4B4B-BA16-BDB2480D6878}" name="Avisos" dataDxfId="22" totalsRowDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{06F20511-43B0-4213-B039-8F04FE3FD409}" name="Produto" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{833D9E07-786D-4F11-ADBE-EB9FE9DA20F3}" name="Medida" dataDxfId="28" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{2E7F5760-F579-440C-BB90-F0ABAA3977A1}" name="Estoque _x000a_Minimo" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{3544D7B8-7225-4D56-B67E-FCBE646D64FA}" name="Estoque _x000a_maximo" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{941540F3-D296-4F60-96B3-0CA20F164402}" name="Saldo " totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="20">
+      <calculatedColumnFormula>SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[entrada])-SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[saida])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{28ED0648-8C45-4B4B-BA16-BDB2480D6878}" name="Avisos" dataDxfId="18" totalsRowDxfId="19">
+      <calculatedColumnFormula>IF(tb_cadastro[[#This Row],[Saldo ]]&lt;tb_cadastro[[#This Row],[Estoque 
+Minimo]],"Priorizar compra Urgente",IF(tb_cadastro[[#This Row],[Saldo ]]&gt;tb_cadastro[[#This Row],[Estoque 
+maximo]],"Priorizar venda",""))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C4BB66EA-2EE0-4143-BBCB-3F4E85542AFC}" name="tb_lancamentos" displayName="tb_lancamentos" ref="A3:E6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="Bom">
-  <autoFilter ref="A3:E5" xr:uid="{C4BB66EA-2EE0-4143-BBCB-3F4E85542AFC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C4BB66EA-2EE0-4143-BBCB-3F4E85542AFC}" name="tb_lancamentos" displayName="tb_lancamentos" ref="A3:E9" totalsRowCount="1" headerRowDxfId="37" dataDxfId="36" headerRowCellStyle="Bom">
+  <autoFilter ref="A3:E8" xr:uid="{C4BB66EA-2EE0-4143-BBCB-3F4E85542AFC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{422F51CF-6BC1-4893-86F3-AF00D407A13B}" name="Produto" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{45889AA7-0406-45FF-BB60-1478B9B496F0}" name="data" dataDxfId="14" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{7853E2EB-0E41-43B4-9FAF-7ECD069304AA}" name="entrada" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6AB0658A-0D59-4B07-9B55-C0F51C18D262}" name="saida" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{54F0E609-B7A0-4EDB-9DE8-3FCDD46F97A9}" name="saldo" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{422F51CF-6BC1-4893-86F3-AF00D407A13B}" name="Produto" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{45889AA7-0406-45FF-BB60-1478B9B496F0}" name="data" dataDxfId="3" totalsRowDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{7853E2EB-0E41-43B4-9FAF-7ECD069304AA}" name="entrada" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{6AB0658A-0D59-4B07-9B55-C0F51C18D262}" name="saida" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{54F0E609-B7A0-4EDB-9DE8-3FCDD46F97A9}" name="saldo" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="31">
+      <calculatedColumnFormula>SUMIFS(tb_lancamentos[entrada],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]]) - SUMIFS(tb_lancamentos[saida],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1652,37 +2950,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E580E2F3-0C79-4348-8AD8-6FA7E4F4392A}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" style="16" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="3" max="5" width="15.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="148.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="0" style="2" hidden="1"/>
+    <col min="8" max="8" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
       <c r="F2"/>
       <c r="G2"/>
     </row>
@@ -1693,13 +2991,13 @@
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1713,14 +3011,22 @@
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>15</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <v>150</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="13">
+        <f>SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[entrada])-SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[saida])</f>
+        <v>65</v>
+      </c>
+      <c r="F4" s="20" t="str">
+        <f>IF(tb_cadastro[[#This Row],[Saldo ]]&lt;tb_cadastro[[#This Row],[Estoque 
+Minimo]],"Priorizar compra Urgente",IF(tb_cadastro[[#This Row],[Saldo ]]&gt;tb_cadastro[[#This Row],[Estoque 
+maximo]],"Priorizar venda",""))</f>
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1729,14 +3035,22 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="13">
         <v>15</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <v>150</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="13">
+        <f>SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[entrada])-SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[saida])</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f>IF(tb_cadastro[[#This Row],[Saldo ]]&lt;tb_cadastro[[#This Row],[Estoque 
+Minimo]],"Priorizar compra Urgente",IF(tb_cadastro[[#This Row],[Saldo ]]&gt;tb_cadastro[[#This Row],[Estoque 
+maximo]],"Priorizar venda",""))</f>
+        <v>Priorizar compra Urgente</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1745,14 +3059,22 @@
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="13">
         <v>15</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>150</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="13">
+        <f>SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[entrada])-SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[saida])</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <f>IF(tb_cadastro[[#This Row],[Saldo ]]&lt;tb_cadastro[[#This Row],[Estoque 
+Minimo]],"Priorizar compra Urgente",IF(tb_cadastro[[#This Row],[Saldo ]]&gt;tb_cadastro[[#This Row],[Estoque 
+maximo]],"Priorizar venda",""))</f>
+        <v>Priorizar compra Urgente</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1761,101 +3083,133 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="13">
         <v>10</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>50</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="13">
+        <f>SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[entrada])-SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[saida])</f>
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="str">
+        <f>IF(tb_cadastro[[#This Row],[Saldo ]]&lt;tb_cadastro[[#This Row],[Estoque 
+Minimo]],"Priorizar compra Urgente",IF(tb_cadastro[[#This Row],[Saldo ]]&gt;tb_cadastro[[#This Row],[Estoque 
+maximo]],"Priorizar venda",""))</f>
+        <v/>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13">
+        <v>20</v>
+      </c>
+      <c r="D8" s="13">
+        <v>55</v>
+      </c>
+      <c r="E8" s="13">
+        <f>SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[entrada])-SUMIF(tb_lancamentos[Produto],tb_cadastro[[#This Row],[Produto]],tb_lancamentos[saida])</f>
+        <v>17</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f>IF(tb_cadastro[[#This Row],[Saldo ]]&lt;tb_cadastro[[#This Row],[Estoque 
+Minimo]],"Priorizar compra Urgente",IF(tb_cadastro[[#This Row],[Saldo ]]&gt;tb_cadastro[[#This Row],[Estoque 
+maximo]],"Priorizar venda",""))</f>
+        <v>Priorizar compra Urgente</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="15">
+      <c r="B9" s="4"/>
+      <c r="C9" s="13">
         <f>SUBTOTAL(109,tb_cadastro[Estoque 
 Minimo])</f>
-        <v>55</v>
-      </c>
-      <c r="D8" s="15">
+        <v>75</v>
+      </c>
+      <c r="D9" s="13">
         <f>SUBTOTAL(109,tb_cadastro[Estoque 
 maximo])</f>
-        <v>500</v>
-      </c>
-      <c r="E8" s="15">
+        <v>555</v>
+      </c>
+      <c r="E9" s="13">
         <f>SUBTOTAL(109,tb_cadastro[[Saldo ]])</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9"/>
+        <v>96</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
       <c r="F13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
       <c r="F14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
       <c r="F15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="F16"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F4:F8">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Priorizar compra Urgente">
+      <formula>NOT(ISERROR(SEARCH("Priorizar compra Urgente",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Priorizar venda">
+      <formula>NOT(ISERROR(SEARCH("Priorizar venda",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1867,18 +3221,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EB24B8-8375-4418-85F5-362D21D0943E}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" style="16" customWidth="1"/>
+    <col min="3" max="5" width="15.7109375" style="14" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="148.140625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2" hidden="1"/>
@@ -1886,10 +3240,10 @@
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
@@ -1897,68 +3251,146 @@
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="23" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="24">
         <v>43698</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>30</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="25">
         <v>5</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="26">
+        <f>SUMIFS(tb_lancamentos[entrada],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]]) - SUMIFS(tb_lancamentos[saida],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]])</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="24">
         <v>44096</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="13">
+        <v>20</v>
+      </c>
+      <c r="D5" s="25">
+        <v>8</v>
+      </c>
+      <c r="E5" s="26">
+        <f>SUMIFS(tb_lancamentos[entrada],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]]) - SUMIFS(tb_lancamentos[saida],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]])</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="24">
+        <v>44492</v>
+      </c>
+      <c r="C6" s="13">
+        <v>5</v>
+      </c>
+      <c r="D6" s="25">
+        <v>3</v>
+      </c>
+      <c r="E6" s="26">
+        <f>SUMIFS(tb_lancamentos[entrada],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]]) - SUMIFS(tb_lancamentos[saida],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="24">
+        <v>44890</v>
+      </c>
+      <c r="C7" s="13">
+        <v>50</v>
+      </c>
+      <c r="D7" s="25">
         <v>10</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="15">
+      <c r="E7" s="26">
+        <f>SUMIFS(tb_lancamentos[entrada],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]]) - SUMIFS(tb_lancamentos[saida],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]])</f>
+        <v>65</v>
+      </c>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="24">
+        <v>44891</v>
+      </c>
+      <c r="C8" s="13">
+        <v>30</v>
+      </c>
+      <c r="D8" s="25">
+        <v>13</v>
+      </c>
+      <c r="E8" s="26">
+        <f>SUMIFS(tb_lancamentos[entrada],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]]) - SUMIFS(tb_lancamentos[saida],tb_lancamentos[Produto],tb_lancamentos[[#This Row],[Produto]],tb_lancamentos[data],"&lt;="&amp;tb_lancamentos[[#This Row],[data]])</f>
+        <v>17</v>
+      </c>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="13">
         <f>SUBTOTAL(109,tb_lancamentos[entrada])</f>
-        <v>30</v>
-      </c>
-      <c r="D6" s="15">
+        <v>135</v>
+      </c>
+      <c r="D9" s="13">
         <f>SUBTOTAL(109,tb_lancamentos[saida])</f>
-        <v>5</v>
-      </c>
-      <c r="E6" s="15">
+        <v>39</v>
+      </c>
+      <c r="E9" s="13">
         <f>SUBTOTAL(109,tb_lancamentos[saldo])</f>
-        <v>0</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A9" xr:uid="{7672FFFC-9048-46E3-B59C-CBABB80E34F2}">
+      <formula1>coluna_produtos</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>